<commit_message>
TEST: Add test results
Add test results for part 2 in excel file
</commit_message>
<xml_diff>
--- a/test-case.xlsx
+++ b/test-case.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\L6\Advance Software Engineering\Assessment\graphical-programming-language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBE7793-1E33-4F34-855B-58EB93B92854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35DA5A5-FDD3-4AAD-B814-72D4DB4A5BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16785" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{6AF5342F-A4B6-4514-A17D-12036C8761EC}"/>
+    <workbookView xWindow="-12195" yWindow="4425" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{6AF5342F-A4B6-4514-A17D-12036C8761EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="ShapeCompiler" sheetId="8" r:id="rId1"/>
-    <sheet name="ShapeFactoryTest" sheetId="10" r:id="rId2"/>
+    <sheet name="ShapeCompilerTest" sheetId="8" r:id="rId1"/>
+    <sheet name="LexerTest" sheetId="11" r:id="rId2"/>
+    <sheet name="ShapeFactoryTest" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="76">
   <si>
     <t>Pass</t>
   </si>
@@ -256,6 +257,127 @@
   </si>
   <si>
     <t>Function runs and generates correct command</t>
+  </si>
+  <si>
+    <t>SC_ParseUsingLexer_003</t>
+  </si>
+  <si>
+    <t>"width = 100\nheight = 100\nwidth = 200", "run"</t>
+  </si>
+  <si>
+    <t>Create an instance of ShapeCompiler</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ParseProgram</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with the test data</t>
+    </r>
+  </si>
+  <si>
+    <t>Function runs and generates tokens</t>
+  </si>
+  <si>
+    <t>SC_AssignVariable_004</t>
+  </si>
+  <si>
+    <t>Test the ParseUsingLexer function of the ShapeCompiler class</t>
+  </si>
+  <si>
+    <t>Test the Variable Assignment feature of the ShapeCompiler class</t>
+  </si>
+  <si>
+    <t>Function runs, generates and assign value to the variable</t>
+  </si>
+  <si>
+    <t>SC_RunLoop_005</t>
+  </si>
+  <si>
+    <t>Test the Looping feature of the ShapeCompiler class</t>
+  </si>
+  <si>
+    <t>"count = 10\nwhile count &gt; 1\ncount = count - 1\nendwhile", "run"</t>
+  </si>
+  <si>
+    <t>Function runs and loop runs correctly</t>
+  </si>
+  <si>
+    <t>SC_IfStatement_006</t>
+  </si>
+  <si>
+    <t>"count = 1\nif count &gt; 0\n count = count + 1\nendif", "run"</t>
+  </si>
+  <si>
+    <t>Function runs and if statement is handeled correctly</t>
+  </si>
+  <si>
+    <t>Test the If conditional statement feature of the ShapeCompiler class</t>
+  </si>
+  <si>
+    <t>L_Advance_001</t>
+  </si>
+  <si>
+    <t>Test function of the Lexer class</t>
+  </si>
+  <si>
+    <t>Access to Lexer class</t>
+  </si>
+  <si>
+    <t>"width = 100"</t>
+  </si>
+  <si>
+    <t>Test the Advance function of the Lexer class</t>
+  </si>
+  <si>
+    <t>Create an instance of Lexer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Advance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with the test data</t>
+    </r>
+  </si>
+  <si>
+    <t>Function runs and returns correct tokens</t>
   </si>
 </sst>
 </file>
@@ -403,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -447,20 +569,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -471,32 +593,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E7896B-39D1-4429-8AB0-C6B1792E0558}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:F36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,10 +1021,10 @@
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -918,15 +1037,15 @@
       <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="1"/>
       <c r="E7" s="20">
         <v>1</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -934,23 +1053,23 @@
       <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="31"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="1"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="29"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -964,13 +1083,13 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -993,17 +1112,17 @@
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
@@ -1011,10 +1130,10 @@
       <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1029,10 +1148,10 @@
       <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1041,8 +1160,8 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1051,8 +1170,8 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1128,10 +1247,10 @@
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
         <v>9</v>
@@ -1144,15 +1263,15 @@
       <c r="A26" s="6">
         <v>1</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="1"/>
       <c r="E26" s="20">
         <v>1</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="23" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1160,23 +1279,23 @@
       <c r="A27" s="6">
         <v>2</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="1"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="31"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>3</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="1"/>
       <c r="E28" s="22"/>
-      <c r="F28" s="29"/>
+      <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -1190,13 +1309,13 @@
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="27"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -1219,17 +1338,17 @@
       <c r="D32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="24"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>19</v>
@@ -1237,10 +1356,10 @@
       <c r="D33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="16"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -1255,10 +1374,10 @@
       <c r="D34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F34" s="16"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1267,8 +1386,8 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -1277,24 +1396,42 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="29"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="14"/>
+      <c r="A39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="7"/>
+      <c r="E40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
@@ -1304,13 +1441,25 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="3"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="4">
+        <v>43933</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -1321,36 +1470,58 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="A44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="15"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="6">
+        <v>1</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="16"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="6"/>
+      <c r="E45" s="20">
+        <v>1</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
+      <c r="A46" s="6">
+        <v>2</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="16"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="6"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
+      <c r="A47" s="3">
+        <v>3</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="6"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="25"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
@@ -1361,12 +1532,16 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="18"/>
+      <c r="A49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>57</v>
+      </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -1376,61 +1551,113 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="27"/>
+    </row>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>1</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="29"/>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>2</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="3">
+        <v>3</v>
+      </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="3">
+        <v>4</v>
+      </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="29"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="14"/>
+      <c r="A58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="7"/>
+      <c r="E59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
@@ -1440,13 +1667,25 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="3"/>
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="4">
+        <v>43933</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
@@ -1457,36 +1696,58 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
+      <c r="A63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="15"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
+      <c r="A64" s="6">
+        <v>1</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="16"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="6"/>
+      <c r="E64" s="20">
+        <v>1</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
+      <c r="A65" s="6">
+        <v>2</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="16"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="6"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="24"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
+      <c r="A66" s="3">
+        <v>3</v>
+      </c>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="6"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="25"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
@@ -1497,12 +1758,16 @@
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="18"/>
+      <c r="A68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="C68" s="18"/>
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
+      <c r="F68" s="19"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
@@ -1512,48 +1777,598 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
+    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="27"/>
+    </row>
+    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>1</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="29"/>
+    </row>
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>2</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F72" s="29"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
+      <c r="A73" s="3">
+        <v>3</v>
+      </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="16"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="29"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
+      <c r="A74" s="3">
+        <v>4</v>
+      </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="16"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="29"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="4">
+        <v>43933</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="15"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>1</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="16"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="20">
+        <v>1</v>
+      </c>
+      <c r="F83" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>2</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" s="16"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="24"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>3</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="25"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="19"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F89" s="27"/>
+    </row>
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>1</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" s="29"/>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>2</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F91" s="29"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>3</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="29"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>4</v>
+      </c>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="29"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F97" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="4">
+        <v>43933</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="15"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
+        <v>1</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="20">
+        <v>1</v>
+      </c>
+      <c r="F102" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>2</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="24"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>3</v>
+      </c>
+      <c r="B104" s="16"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="25"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="19"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F108" s="27"/>
+    </row>
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <v>1</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E109" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F109" s="29"/>
+    </row>
+    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
+        <v>2</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F110" s="29"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>3</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="29"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>4</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="78">
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="E83:E85"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="D39:F39"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B6:C6"/>
@@ -1568,50 +2383,280 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D3B562-F25C-461D-80CC-00D9C9A4E8DF}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43933</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="20">
+        <v>1</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="29"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="29"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57857961-BFDD-4435-BC75-7D54FF35CFE7}">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="A58" sqref="A58:F74"/>
     </sheetView>
   </sheetViews>
@@ -1699,10 +2744,10 @@
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -1715,15 +2760,15 @@
       <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="1"/>
       <c r="E7" s="20">
         <v>1</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1731,23 +2776,23 @@
       <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="31"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="1"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="29"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1761,13 +2806,13 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1790,10 +2835,10 @@
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1808,10 +2853,10 @@
       <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1826,10 +2871,10 @@
       <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1838,8 +2883,8 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1848,8 +2893,8 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1925,10 +2970,10 @@
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
         <v>9</v>
@@ -1941,15 +2986,15 @@
       <c r="A26" s="6">
         <v>1</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="1"/>
       <c r="E26" s="20">
         <v>1</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="23" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1957,23 +3002,23 @@
       <c r="A27" s="6">
         <v>2</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="1"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="31"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>3</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="1"/>
       <c r="E28" s="22"/>
-      <c r="F28" s="29"/>
+      <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -1987,13 +3032,13 @@
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="27"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -2016,10 +3061,10 @@
       <c r="D32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="24"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -2034,10 +3079,10 @@
       <c r="D33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="16"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -2052,10 +3097,10 @@
       <c r="D34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F34" s="16"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -2064,8 +3109,8 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -2074,8 +3119,8 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="29"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -2151,10 +3196,10 @@
       <c r="A44" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="19"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="1"/>
       <c r="E44" s="2" t="s">
         <v>9</v>
@@ -2167,15 +3212,15 @@
       <c r="A45" s="6">
         <v>1</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="1"/>
       <c r="E45" s="20">
         <v>1</v>
       </c>
-      <c r="F45" s="30" t="s">
+      <c r="F45" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2183,23 +3228,23 @@
       <c r="A46" s="6">
         <v>2</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="1"/>
       <c r="E46" s="21"/>
-      <c r="F46" s="31"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>3</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="1"/>
       <c r="E47" s="22"/>
-      <c r="F47" s="29"/>
+      <c r="F47" s="25"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
@@ -2213,13 +3258,13 @@
       <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="27"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -2242,10 +3287,10 @@
       <c r="D51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="24"/>
+      <c r="F51" s="27"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
@@ -2260,10 +3305,10 @@
       <c r="D52" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F52" s="16"/>
+      <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -2278,10 +3323,10 @@
       <c r="D53" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F53" s="16"/>
+      <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
@@ -2290,8 +3335,8 @@
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -2300,8 +3345,8 @@
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="29"/>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -2377,10 +3422,10 @@
       <c r="A63" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="19"/>
+      <c r="C63" s="15"/>
       <c r="D63" s="1"/>
       <c r="E63" s="2" t="s">
         <v>9</v>
@@ -2393,15 +3438,15 @@
       <c r="A64" s="6">
         <v>1</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="17"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="1"/>
       <c r="E64" s="20">
         <v>1</v>
       </c>
-      <c r="F64" s="30" t="s">
+      <c r="F64" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2409,23 +3454,23 @@
       <c r="A65" s="6">
         <v>2</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="17"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="1"/>
       <c r="E65" s="21"/>
-      <c r="F65" s="31"/>
+      <c r="F65" s="24"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>3</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="1"/>
       <c r="E66" s="22"/>
-      <c r="F66" s="29"/>
+      <c r="F66" s="25"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
@@ -2439,13 +3484,13 @@
       <c r="A68" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B68" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="27"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="19"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
@@ -2468,10 +3513,10 @@
       <c r="D70" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="23" t="s">
+      <c r="E70" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F70" s="24"/>
+      <c r="F70" s="27"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
@@ -2486,10 +3531,10 @@
       <c r="D71" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E71" s="15" t="s">
+      <c r="E71" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F71" s="16"/>
+      <c r="F71" s="29"/>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
@@ -2504,10 +3549,10 @@
       <c r="D72" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E72" s="15" t="s">
+      <c r="E72" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F72" s="16"/>
+      <c r="F72" s="29"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
@@ -2516,8 +3561,8 @@
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="16"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="29"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
@@ -2526,16 +3571,16 @@
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="16"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="29"/>
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="16"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="29"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
@@ -2571,32 +3616,32 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
       <c r="D82" s="1"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
       <c r="D83" s="1"/>
       <c r="E83" s="11"/>
       <c r="F83" s="8"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
       <c r="D84" s="1"/>
       <c r="E84" s="12"/>
       <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
       <c r="D85" s="1"/>
       <c r="E85" s="13"/>
       <c r="F85" s="10"/>
@@ -2611,11 +3656,11 @@
     </row>
     <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="27"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="19"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
@@ -2630,48 +3675,48 @@
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="24"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="27"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="16"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="29"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
-      <c r="E91" s="15"/>
-      <c r="F91" s="16"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="29"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
-      <c r="E92" s="15"/>
-      <c r="F92" s="16"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="29"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="16"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="29"/>
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="16"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="30"/>
+      <c r="F96" s="29"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
@@ -2707,32 +3752,32 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="15"/>
       <c r="D101" s="1"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
+      <c r="B102" s="16"/>
+      <c r="C102" s="16"/>
       <c r="D102" s="1"/>
       <c r="E102" s="11"/>
       <c r="F102" s="8"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="16"/>
       <c r="D103" s="1"/>
       <c r="E103" s="12"/>
       <c r="F103" s="9"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="16"/>
       <c r="D104" s="1"/>
       <c r="E104" s="13"/>
       <c r="F104" s="10"/>
@@ -2747,11 +3792,11 @@
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
-      <c r="B106" s="25"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="27"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="19"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
@@ -2766,56 +3811,56 @@
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="23"/>
-      <c r="F108" s="24"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="27"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
-      <c r="E109" s="15"/>
-      <c r="F109" s="16"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="29"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
-      <c r="E110" s="15"/>
-      <c r="F110" s="16"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="29"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
-      <c r="E111" s="15"/>
-      <c r="F111" s="16"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="29"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="16"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="29"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
-      <c r="E113" s="15"/>
-      <c r="F113" s="16"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="29"/>
     </row>
     <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="16"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="30"/>
+      <c r="F116" s="29"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
@@ -2851,32 +3896,32 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
-      <c r="B121" s="19"/>
-      <c r="C121" s="19"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="15"/>
       <c r="D121" s="1"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
+      <c r="B122" s="16"/>
+      <c r="C122" s="16"/>
       <c r="D122" s="1"/>
       <c r="E122" s="11"/>
       <c r="F122" s="8"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
+      <c r="B123" s="16"/>
+      <c r="C123" s="16"/>
       <c r="D123" s="1"/>
       <c r="E123" s="12"/>
       <c r="F123" s="9"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="17"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
       <c r="D124" s="1"/>
       <c r="E124" s="13"/>
       <c r="F124" s="10"/>
@@ -2891,11 +3936,11 @@
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
-      <c r="B126" s="25"/>
-      <c r="C126" s="26"/>
-      <c r="D126" s="26"/>
-      <c r="E126" s="26"/>
-      <c r="F126" s="27"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="18"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="19"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
@@ -2910,56 +3955,56 @@
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
-      <c r="E128" s="23"/>
-      <c r="F128" s="24"/>
+      <c r="E128" s="26"/>
+      <c r="F128" s="27"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
-      <c r="E129" s="15"/>
-      <c r="F129" s="16"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="29"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
-      <c r="E130" s="15"/>
-      <c r="F130" s="16"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="29"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
-      <c r="E131" s="15"/>
-      <c r="F131" s="16"/>
+      <c r="E131" s="28"/>
+      <c r="F131" s="29"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
-      <c r="E132" s="15"/>
-      <c r="F132" s="16"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="29"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
-      <c r="E133" s="15"/>
-      <c r="F133" s="16"/>
+      <c r="E133" s="28"/>
+      <c r="F133" s="29"/>
     </row>
     <row r="136" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="2"/>
-      <c r="D136" s="15"/>
-      <c r="E136" s="28"/>
-      <c r="F136" s="16"/>
+      <c r="D136" s="28"/>
+      <c r="E136" s="30"/>
+      <c r="F136" s="29"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
@@ -2995,32 +4040,32 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
-      <c r="B141" s="19"/>
-      <c r="C141" s="19"/>
+      <c r="B141" s="15"/>
+      <c r="C141" s="15"/>
       <c r="D141" s="1"/>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
-      <c r="B142" s="17"/>
-      <c r="C142" s="17"/>
+      <c r="B142" s="16"/>
+      <c r="C142" s="16"/>
       <c r="D142" s="1"/>
       <c r="E142" s="11"/>
       <c r="F142" s="8"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
-      <c r="B143" s="17"/>
-      <c r="C143" s="17"/>
+      <c r="B143" s="16"/>
+      <c r="C143" s="16"/>
       <c r="D143" s="1"/>
       <c r="E143" s="12"/>
       <c r="F143" s="9"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
-      <c r="B144" s="17"/>
-      <c r="C144" s="17"/>
+      <c r="B144" s="16"/>
+      <c r="C144" s="16"/>
       <c r="D144" s="1"/>
       <c r="E144" s="13"/>
       <c r="F144" s="10"/>
@@ -3035,11 +4080,11 @@
     </row>
     <row r="146" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
-      <c r="B146" s="25"/>
-      <c r="C146" s="26"/>
-      <c r="D146" s="26"/>
-      <c r="E146" s="26"/>
-      <c r="F146" s="27"/>
+      <c r="B146" s="17"/>
+      <c r="C146" s="18"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="18"/>
+      <c r="F146" s="19"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
@@ -3054,74 +4099,115 @@
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="23"/>
-      <c r="F148" s="24"/>
+      <c r="E148" s="26"/>
+      <c r="F148" s="27"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
-      <c r="E149" s="15"/>
-      <c r="F149" s="16"/>
+      <c r="E149" s="28"/>
+      <c r="F149" s="29"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="16"/>
+      <c r="E150" s="28"/>
+      <c r="F150" s="29"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
-      <c r="E151" s="15"/>
-      <c r="F151" s="16"/>
+      <c r="E151" s="28"/>
+      <c r="F151" s="29"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="16"/>
+      <c r="E152" s="28"/>
+      <c r="F152" s="29"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="16"/>
+      <c r="E153" s="28"/>
+      <c r="F153" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="E129:F129"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E150:F150"/>
+    <mergeCell ref="E151:F151"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="E153:F153"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="E148:F148"/>
+    <mergeCell ref="E149:F149"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="E131:F131"/>
+    <mergeCell ref="E132:F132"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="D136:F136"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="B25:C25"/>
@@ -3134,70 +4220,29 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="E131:F131"/>
-    <mergeCell ref="E132:F132"/>
-    <mergeCell ref="E133:F133"/>
-    <mergeCell ref="D136:F136"/>
-    <mergeCell ref="E150:F150"/>
-    <mergeCell ref="E151:F151"/>
-    <mergeCell ref="E152:F152"/>
-    <mergeCell ref="E153:F153"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="E148:F148"/>
-    <mergeCell ref="E149:F149"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="E129:F129"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>